<commit_message>
daha once gidilen konumlar icin hashmap kullanildi
</commit_message>
<xml_diff>
--- a/GANTT CHART.xlsx
+++ b/GANTT CHART.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\behlul\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\behlul\Desktop\BitirmeProjesi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F797E63-88E2-497A-9595-A6BBD870843C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F679A8D1-A2BF-4718-AAC5-12BD08E6E8D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Görev</t>
   </si>
@@ -71,13 +71,19 @@
   <si>
     <t>Hayaletler için kullanılacak stratejilerin belirlenmesi</t>
   </si>
+  <si>
+    <t>Önceki yarışmaların incelenmesi</t>
+  </si>
+  <si>
+    <t>Ms. Pac-Man oyununun araştırılması</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -172,7 +178,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -194,7 +200,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="tr-TR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -276,37 +282,43 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sayfa1!$A$2:$A$11</c:f>
+              <c:f>Sayfa1!$A$2:$A$13</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>Proje konusunun kesinleştirilmesi</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Ms. Pac-Man oyununun araştırılması</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Yarışma tarafından sağlanan paketlerin incelenmesi</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>Önceki yarışmaların incelenmesi</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>Akıllı algoritmaların araştırılması</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>İhtiyaç analizi</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>"Use Case" diagramlarının oluşturulması</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>Ms. Pac-Man ve hayaletler için kullanılacak stratejinin belirlenmesi</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>Hayaletler için kullanılacak stratejilerin belirlenmesi</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>Yazılımın geliştirilmesi</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>Test aşaması ve sonuçların değerlendirilmesi</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>Dökümanların hazırlanması</c:v>
                 </c:pt>
               </c:strCache>
@@ -314,39 +326,45 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sayfa1!$B$2:$B$11</c:f>
+              <c:f>Sayfa1!$B$2:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yy;@</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>43724</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43738</c:v>
+                  <c:v>43731</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43788</c:v>
+                  <c:v>43759</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43828</c:v>
+                  <c:v>43801</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43848</c:v>
+                  <c:v>43822</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43868</c:v>
+                  <c:v>43843</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43883</c:v>
+                  <c:v>43864</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43913</c:v>
+                  <c:v>43885</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43973</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43983</c:v>
+                  <c:v>43934</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43990</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -384,39 +402,45 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sayfa1!$C$2:$C$11</c:f>
+              <c:f>Sayfa1!$C$2:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>60</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12</c:v>
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1138,13 +1162,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>38098</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>57149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1436,10 +1460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1468,126 +1492,150 @@
         <v>43724</v>
       </c>
       <c r="C2" s="3">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B3" s="4">
-        <f>B2+C2</f>
-        <v>43738</v>
+        <f>B2 + C2</f>
+        <v>43731</v>
       </c>
       <c r="C3" s="3">
-        <v>50</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4">
-        <f>B3+C3</f>
-        <v>43788</v>
+        <f t="shared" ref="B4:B13" si="0">B3 + C3</f>
+        <v>43759</v>
       </c>
       <c r="C4" s="3">
-        <v>40</v>
-      </c>
-      <c r="G4" s="1"/>
+        <v>42</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4">
-        <f>B4+C4</f>
-        <v>43828</v>
+        <f t="shared" si="0"/>
+        <v>43801</v>
       </c>
       <c r="C5" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="4">
-        <f>B5+C5</f>
-        <v>43848</v>
+        <f t="shared" si="0"/>
+        <v>43822</v>
       </c>
       <c r="C6" s="3">
-        <v>20</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="4">
-        <f>B6+C6</f>
-        <v>43868</v>
+        <f t="shared" si="0"/>
+        <v>43843</v>
       </c>
       <c r="C7" s="3">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="4">
-        <f>B7+C7</f>
-        <v>43883</v>
+        <f t="shared" si="0"/>
+        <v>43864</v>
       </c>
       <c r="C8" s="3">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="4">
-        <f>B8+C8</f>
-        <v>43913</v>
+        <f t="shared" si="0"/>
+        <v>43885</v>
       </c>
       <c r="C9" s="3">
-        <v>60</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B10" s="4">
-        <f>B9+C9</f>
-        <v>43973</v>
+        <f t="shared" si="0"/>
+        <v>43899</v>
       </c>
       <c r="C10" s="3">
-        <v>10</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B11" s="4">
-        <f>B10+C10</f>
-        <v>43983</v>
+        <f t="shared" si="0"/>
+        <v>43934</v>
       </c>
       <c r="C11" s="3">
-        <v>12</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E12" s="1"/>
+      <c r="A12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="4">
+        <f t="shared" si="0"/>
+        <v>43990</v>
+      </c>
+      <c r="C12" s="3">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="4">
+        <f t="shared" si="0"/>
+        <v>44004</v>
+      </c>
+      <c r="C13" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="1">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
         <v>43724</v>
       </c>
     </row>

</xml_diff>